<commit_message>
fix: fixed == delims
</commit_message>
<xml_diff>
--- a/Files/cfg/first_set.xlsx
+++ b/Files/cfg/first_set.xlsx
@@ -457,7 +457,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>&lt;program&gt;</t>
+          <t>First(&lt;program&gt;)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'shimenet', 'anda', 'andamhie', 'chika', 'naur', 'eklabool'}</t>
+          <t>{'chika', 'shimenet', 'naur', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>&lt;global-dec&gt;</t>
+          <t>First(&lt;global-dec&gt;)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'λ', 'shimenet', 'anda', 'andamhie', 'chika', 'naur', 'eklabool'}</t>
+          <t>{'chika', 'λ', 'shimenet', 'eklabool', 'naur', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>&lt;var-dec-init&gt;</t>
+          <t>First(&lt;var-dec-init&gt;)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'λ', 'shimenet', 'anda', 'andamhie', 'chika', 'naur', 'eklabool'}</t>
+          <t>{'chika', 'λ', 'shimenet', 'naur', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>&lt;naur-case&gt;</t>
+          <t>First(&lt;naur-case&gt;)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>&lt;return-type&gt;</t>
+          <t>First(&lt;return-type&gt;)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'eklabool', 'shimenet', 'anda', 'andamhie', 'chika'}</t>
+          <t>{'shimenet', 'eklabool', 'anda', 'andamhie', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>&lt;data-type&gt;</t>
+          <t>First(&lt;data-type&gt;)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{'eklabool', 'andamhie', 'chika', 'anda'}</t>
+          <t>{'anda', 'eklabool', 'andamhie', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>&lt;func-array-init-tail&gt;</t>
+          <t>First(&lt;func-array-init-tail&gt;)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{'[', '=', '('}</t>
+          <t>{'[', '(', '='}</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>&lt;func-case&gt;</t>
+          <t>First(&lt;func-case&gt;)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -617,7 +617,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>&lt;parameters&gt;</t>
+          <t>First(&lt;parameters&gt;)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{'λ', 'anda', 'andamhie', 'chika', 'eklabool'}</t>
+          <t>{'λ', 'chika', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>&lt;func-parameters&gt;</t>
+          <t>First(&lt;func-parameters&gt;)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -647,7 +647,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{'eklabool', 'andamhie', 'chika', 'anda'}</t>
+          <t>{'anda', 'chika', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>&lt;multi-parameters&gt;</t>
+          <t>First(&lt;multi-parameters&gt;)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>&lt;array-case&gt;</t>
+          <t>First(&lt;array-case&gt;)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -697,7 +697,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>&lt;2d-index&gt;</t>
+          <t>First(&lt;2d-index&gt;)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>&lt;3d-index&gt;</t>
+          <t>First(&lt;3d-index&gt;)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>&lt;array-values&gt;</t>
+          <t>First(&lt;array-values&gt;)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>&lt;literals&gt;</t>
+          <t>First(&lt;literals&gt;)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{'andamhie_literal', 'chika_literal', 'eme', 'korik', 'anda_literal'}</t>
+          <t>{'chika_literal', 'anda_literal', 'korik', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>&lt;eklabool&gt;</t>
+          <t>First(&lt;eklabool&gt;)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{'eme', 'korik'}</t>
+          <t>{'korik', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>&lt;func-array&gt;</t>
+          <t>First(&lt;func-array&gt;)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>&lt;func-array-value&gt;</t>
+          <t>First(&lt;func-array-value&gt;)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{'[', 'λ', '('}</t>
+          <t>{'[', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>&lt;var-init&gt;</t>
+          <t>First(&lt;var-init&gt;)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -857,7 +857,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>&lt;var-init-tail&gt;</t>
+          <t>First(&lt;var-init-tail&gt;)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>&lt;multi-init-values&gt;</t>
+          <t>First(&lt;multi-init-values&gt;)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>&lt;multi-init-values-tail&gt;</t>
+          <t>First(&lt;multi-init-values-tail&gt;)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>&lt;init-values&gt;</t>
+          <t>First(&lt;init-values&gt;)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>&lt;array-init&gt;</t>
+          <t>First(&lt;array-init&gt;)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>&lt;array-elements&gt;</t>
+          <t>First(&lt;array-elements&gt;)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', '{', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme', '{'}</t>
         </is>
       </c>
     </row>
@@ -977,7 +977,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>&lt;2d-array-elements&gt;</t>
+          <t>First(&lt;2d-array-elements&gt;)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'λ', 'id', '-', 'andamhie_literal', 'anda_literal', '{', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', 'λ', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme', '{'}</t>
         </is>
       </c>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>&lt;extra-array-value&gt;</t>
+          <t>First(&lt;extra-array-value&gt;)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>&lt;extra-2d-array-value&gt;</t>
+          <t>First(&lt;extra-2d-array-value&gt;)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>&lt;extra-3d-array-value&gt;</t>
+          <t>First(&lt;extra-3d-array-value&gt;)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'λ', 'id', '-', 'andamhie_literal', 'anda_literal', '{', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', 'λ', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme', '{'}</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>&lt;func-def&gt;</t>
+          <t>First(&lt;func-def&gt;)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>{'eklabool', 'λ', 'shimenet', 'anda', 'andamhie', 'chika'}</t>
+          <t>{'shimenet', 'λ', 'eklabool', 'anda', 'andamhie', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>&lt;func-body&gt;</t>
+          <t>First(&lt;func-body&gt;)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++'}</t>
+          <t>{'serve', '++', 'versa', 'keri', 'forda', 'id', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>&lt;multi-statements&gt;</t>
+          <t>First(&lt;multi-statements&gt;)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'eklabool', 'pak', '--', 'push', 'keri', 'anda', 'id', 'andamhie', 'versa', 'serve', '++'}</t>
+          <t>{'serve', '++', 'versa', 'keri', 'forda', 'id', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>&lt;local-dec&gt;</t>
+          <t>First(&lt;local-dec&gt;)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>{'eklabool', 'λ', 'anda', 'andamhie', 'chika', 'naur'}</t>
+          <t>{'λ', 'eklabool', 'naur', 'anda', 'andamhie', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>&lt;local-dec-init&gt;</t>
+          <t>First(&lt;local-dec-init&gt;)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>{'anda', 'andamhie', 'chika', 'naur', 'eklabool'}</t>
+          <t>{'chika', 'naur', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>&lt;arguments&gt;</t>
+          <t>First(&lt;arguments&gt;)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'λ', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', 'λ', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>&lt;multi-arguments-value&gt;</t>
+          <t>First(&lt;multi-arguments-value&gt;)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>&lt;arguments-value&gt;</t>
+          <t>First(&lt;arguments-value&gt;)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>&lt;array-assign&gt;</t>
+          <t>First(&lt;array-assign&gt;)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>&lt;kween-body&gt;</t>
+          <t>First(&lt;kween-body&gt;)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>{'λ', 'anda', 'andamhie', 'forda', 'id', 'chika', 'versa', 'naur', 'eklabool', 'pak', 'serve', '++', '--', 'push', 'keri'}</t>
+          <t>{'pak', 'id', 'serve', '++', 'chika', '--', 'λ', 'versa', 'keri', 'eklabool', 'forda', 'push', 'anda', 'naur', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>&lt;expression&gt;</t>
+          <t>First(&lt;expression&gt;)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>&lt;simple-expression&gt;</t>
+          <t>First(&lt;simple-expression&gt;)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>&lt;multi-expression&gt;</t>
+          <t>First(&lt;multi-expression&gt;)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>&lt;expression-tail&gt;</t>
+          <t>First(&lt;expression-tail&gt;)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>{'λ', '&amp;&amp;', '**', '//', '&gt;', '||', '==', '!', '&gt;=', '%', '+', '-', '&lt;=', '*', '&lt;', '/', '=', '+=', '!='}</t>
+          <t>{'&gt;', '&lt;=', '||', '==', '!', '-', '!=', '&lt;', '**', '=', '&amp;&amp;', '+', '+=', 'λ', '&gt;=', '//', '%', '/', '*'}</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>&lt;expression-operands&gt;</t>
+          <t>First(&lt;expression-operands&gt;)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>&lt;negative-value&gt;</t>
+          <t>First(&lt;negative-value&gt;)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>{'-', 'λ'}</t>
+          <t>{'λ', '-'}</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>&lt;expression-value&gt;</t>
+          <t>First(&lt;expression-value&gt;)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'korik', '++', '--', 'eme', 'anda_literal', '(', 'chika_literal', 'id', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>&lt;identifier-tail&gt;</t>
+          <t>First(&lt;identifier-tail&gt;)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>{'[', 'λ', '++', '--', '('}</t>
+          <t>{'[', '(', '--', '++', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>&lt;unary-operator&gt;</t>
+          <t>First(&lt;unary-operator&gt;)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>&lt;general-operands&gt;</t>
+          <t>First(&lt;general-operands&gt;)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>{'anda_literal', 'eme', 'chika_literal', 'korik', 'andamhie_literal'}</t>
+          <t>{'chika_literal', 'anda_literal', 'korik', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>&lt;general-operators&gt;</t>
+          <t>First(&lt;general-operators&gt;)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>{'%', '&amp;&amp;', '**', '+', '-', '&lt;=', '//', '&gt;', '||', '*', '==', '&lt;', '=', '!', '/', '&gt;=', '+=', '!='}</t>
+          <t>{'&gt;', '&amp;&amp;', '&lt;=', '&lt;', '+', '||', '+=', '==', '!', '-', '!=', '&gt;=', '//', '**', '%', '/', '=', '*'}</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>&lt;statements&gt;</t>
+          <t>First(&lt;statements&gt;)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1487,7 +1487,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'eklabool', 'pak', '--', 'push', 'keri', 'anda', 'id', 'andamhie', 'versa', 'serve', '++'}</t>
+          <t>{'serve', '++', 'versa', 'keri', 'forda', 'id', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>&lt;loop-body&gt;</t>
+          <t>First(&lt;loop-body&gt;)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'eklabool', 'pak', 'gogogo', '--', 'push', 'keri', 'anda', 'id', 'andamhie', 'versa', 'serve', '++', 'amaccana'}</t>
+          <t>{'amaccana', 'serve', '++', 'versa', 'keri', 'forda', 'id', 'gogogo', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>&lt;multi-loop-body&gt;</t>
+          <t>First(&lt;multi-loop-body&gt;)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'eklabool', 'pak', 'gogogo', '--', 'push', 'keri', 'anda', 'id', 'andamhie', 'versa', 'serve', '++', 'amaccana'}</t>
+          <t>{'amaccana', 'serve', '++', 'versa', 'keri', 'forda', 'id', 'gogogo', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>&lt;assign-stmts&gt;</t>
+          <t>First(&lt;assign-stmts&gt;)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>{'%', '[', '**', '+', '-', '//', '*', '/', '=', '('}</t>
+          <t>{'+', '-', '[', '(', '//', '**', '%', '/', '=', '*'}</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>&lt;arithmetic-operators&gt;</t>
+          <t>First(&lt;arithmetic-operators&gt;)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>{'%', '*', 'λ', '**', '+', '-', '/', '//'}</t>
+          <t>{'λ', '*', '//', '+', '**', '%', '/', '-'}</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>&lt;assignment-values&gt;</t>
+          <t>First(&lt;assignment-values&gt;)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>&lt;input-stmts&gt;</t>
+          <t>First(&lt;input-stmts&gt;)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>{'eklabool', 'anda', 'andamhie', 'chika', 'id'}</t>
+          <t>{'id', 'eklabool', 'anda', 'andamhie', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>&lt;input-type&gt;</t>
+          <t>First(&lt;input-type&gt;)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>{'λ', 'anda', 'andamhie', 'chika', 'eklabool'}</t>
+          <t>{'chika', 'λ', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>&lt;givenchy-values&gt;</t>
+          <t>First(&lt;givenchy-values&gt;)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>&lt;output-stmts&gt;</t>
+          <t>First(&lt;output-stmts&gt;)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>&lt;output-values&gt;</t>
+          <t>First(&lt;output-values&gt;)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>&lt;conditional-stmts&gt;</t>
+          <t>First(&lt;conditional-stmts&gt;)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>&lt;condition&gt;</t>
+          <t>First(&lt;condition&gt;)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>&lt;conditional-body&gt;</t>
+          <t>First(&lt;conditional-body&gt;)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++'}</t>
+          <t>{'serve', '++', 'versa', 'keri', 'forda', 'id', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>&lt;loop-conditional-stmts&gt;</t>
+          <t>First(&lt;loop-conditional-stmts&gt;)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>&lt;loop-conditional-body&gt;</t>
+          <t>First(&lt;loop-conditional-body&gt;)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', 'gogogo', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++', 'amaccana'}</t>
+          <t>{'amaccana', 'serve', '++', 'versa', 'keri', 'forda', 'id', 'gogogo', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>&lt;ganern-pak-statement&gt;</t>
+          <t>First(&lt;ganern-pak-statement&gt;)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>{'λ', 'ganern'}</t>
+          <t>{'ganern', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>&lt;ganern-case&gt;</t>
+          <t>First(&lt;ganern-case&gt;)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>{'λ', 'ganern'}</t>
+          <t>{'ganern', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>&lt;loop-stmts&gt;</t>
+          <t>First(&lt;loop-stmts&gt;)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>{'forda', 'keri'}</t>
+          <t>{'keri', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>&lt;forda-statement&gt;</t>
+          <t>First(&lt;forda-statement&gt;)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>&lt;loop-type-init&gt;</t>
+          <t>First(&lt;loop-type-init&gt;)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1887,7 +1887,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>{'λ', 'anda', 'andamhie', 'chika', 'eklabool'}</t>
+          <t>{'chika', 'λ', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>&lt;start-value&gt;</t>
+          <t>First(&lt;start-value&gt;)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>&lt;end-value&gt;</t>
+          <t>First(&lt;end-value&gt;)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>&lt;step-case&gt;</t>
+          <t>First(&lt;step-case&gt;)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>&lt;update&gt;</t>
+          <t>First(&lt;update&gt;)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'λ', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', 'λ', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>&lt;loop-conditions&gt;</t>
+          <t>First(&lt;loop-conditions&gt;)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>&lt;for-loop-body&gt;</t>
+          <t>First(&lt;for-loop-body&gt;)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2007,7 +2007,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', 'gogogo', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++', 'amaccana'}</t>
+          <t>{'amaccana', 'serve', '++', 'versa', 'keri', 'forda', 'id', 'gogogo', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>&lt;keri-statement&gt;</t>
+          <t>First(&lt;keri-statement&gt;)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>&lt;keri-case&gt;</t>
+          <t>First(&lt;keri-case&gt;)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>&lt;while-loop-body&gt;</t>
+          <t>First(&lt;while-loop-body&gt;)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', 'gogogo', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++', 'amaccana'}</t>
+          <t>{'amaccana', 'serve', '++', 'versa', 'keri', 'forda', 'id', 'gogogo', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>&lt;switch-stmts&gt;</t>
+          <t>First(&lt;switch-stmts&gt;)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>&lt;multi-cases&gt;</t>
+          <t>First(&lt;multi-cases&gt;)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>{'betsung', 'λ'}</t>
+          <t>{'λ', 'betsung'}</t>
         </is>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>&lt;switch-values&gt;</t>
+          <t>First(&lt;switch-values&gt;)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>&lt;switch-statements&gt;</t>
+          <t>First(&lt;switch-statements&gt;)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++'}</t>
+          <t>{'serve', '++', 'versa', 'keri', 'forda', 'id', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>&lt;loop-switch-stmts&gt;</t>
+          <t>First(&lt;loop-switch-stmts&gt;)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>&lt;loop-multi-cases&gt;</t>
+          <t>First(&lt;loop-multi-cases&gt;)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>{'betsung', 'λ'}</t>
+          <t>{'λ', 'betsung'}</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>&lt;loop-switch-statements&gt;</t>
+          <t>First(&lt;loop-switch-statements&gt;)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>{'λ', 'forda', 'chika', 'naur', 'eklabool', 'pak', 'gogogo', '--', 'push', 'keri', 'anda', 'andamhie', 'id', 'versa', 'serve', '++', 'amaccana'}</t>
+          <t>{'amaccana', 'serve', '++', 'versa', 'keri', 'forda', 'id', 'gogogo', 'andamhie', 'pak', 'chika', '--', 'λ', 'eklabool', 'naur', 'push', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>&lt;amaccana-case&gt;</t>
+          <t>First(&lt;amaccana-case&gt;)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>{'λ', 'amaccana'}</t>
+          <t>{'amaccana', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>&lt;ditech-case&gt;</t>
+          <t>First(&lt;ditech-case&gt;)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>&lt;control-flow-stmts&gt;</t>
+          <t>First(&lt;control-flow-stmts&gt;)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>{'λ', 'gogogo', 'amaccana'}</t>
+          <t>{'amaccana', 'gogogo', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>&lt;return-stmts&gt;</t>
+          <t>First(&lt;return-stmts&gt;)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>{'push', 'λ'}</t>
+          <t>{'λ', 'push'}</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>&lt;unary-stmts&gt;</t>
+          <t>First(&lt;unary-stmts&gt;)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>{'++', '--', 'id'}</t>
+          <t>{'id', '++', '--'}</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>&lt;push-values&gt;</t>
+          <t>First(&lt;push-values&gt;)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2327,7 +2327,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'λ', 'id', '-', 'andamhie_literal', 'anda_literal', 'korik', '++', '--', '('}</t>
+          <t>{'id', 'korik', '++', '--', 'λ', '-', '(', 'chika_literal', 'anda_literal', 'andamhie_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -2335,7 +2335,11 @@
       <c r="A96" t="n">
         <v>95</v>
       </c>
-      <c r="B96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>First()</t>
+        </is>
+      </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>-&gt;</t>

</xml_diff>

<commit_message>
feat: len using string as argument
</commit_message>
<xml_diff>
--- a/Files/cfg/first_set.xlsx
+++ b/Files/cfg/first_set.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'shimenet', 'andamhie', 'chika', 'naur', 'eklabool', 'anda'}</t>
+          <t>{'shimenet', 'naur', 'andamhie', 'anda', 'chika', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'shimenet', 'andamhie', 'naur', 'anda', 'eklabool', 'λ', 'chika'}</t>
+          <t>{'shimenet', 'naur', 'andamhie', 'anda', 'chika', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'shimenet', 'andamhie', 'chika', 'naur', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'shimenet', 'naur', 'andamhie', 'anda', 'chika', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'shimenet', 'andamhie', 'anda', 'eklabool', 'chika'}</t>
+          <t>{'andamhie', 'shimenet', 'anda', 'chika', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{'chika', 'andamhie', 'anda', 'eklabool'}</t>
+          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{'andamhie', 'chika', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'chika', 'andamhie', 'anda', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
+          <t>{'andamhie', 'eklabool', 'anda', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{',', 'λ'}</t>
+          <t>{'λ', ','}</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{'anda_literal', 'chika_literal', 'korik', 'eme', 'andamhie_literal'}</t>
+          <t>{'andamhie_literal', 'chika_literal', 'korik', 'eme', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>{'korik', 'eme'}</t>
+          <t>{'eme', 'korik'}</t>
         </is>
       </c>
     </row>
@@ -907,7 +907,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>{',', 'λ'}</t>
+          <t>{'λ', ','}</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -987,7 +987,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', '{', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '{', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>{',', 'λ'}</t>
+          <t>{'λ', ','}</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>{'andamhie', 'eklabool', 'shimenet', 'chika', 'λ', 'anda'}</t>
+          <t>{'shimenet', 'andamhie', 'anda', 'chika', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>{'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>{'andamhie', 'naur', 'anda', 'eklabool', 'λ', 'chika'}</t>
+          <t>{'andamhie', 'naur', 'anda', 'chika', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>{'andamhie', 'chika', 'naur', 'eklabool', 'anda'}</t>
+          <t>{'naur', 'andamhie', 'anda', 'chika', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'λ', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', 'λ', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>{',', 'λ'}</t>
+          <t>{'λ', ','}</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>{'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'id', 'serve', 'pak', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'andamhie', 'anda', 'keri', 'versa', 'forda', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>{'==', '-', '&amp;&amp;', '&lt;=', '%', '*', '//', '||', '!=', '&gt;', '/', '+', '&gt;=', '&lt;', 'λ', '**'}</t>
+          <t>{'*', '+', '&gt;=', '/', '==', '%', '&lt;=', 'λ', '//', '**', '&gt;', '!=', '&amp;&amp;', '-', '&lt;', '||'}</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>{'-', 'λ', '!'}</t>
+          <t>{'-', '!', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>{'id', 'anda_literal', 'chika_literal', 'korik', 'eme', 'len', '(', '--', '++', 'andamhie_literal'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', 'chika_literal', '--', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>{'(', '[', '--', '++', 'λ'}</t>
+          <t>{'(', '[', '++', '--', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>{'anda_literal', 'chika_literal', 'andamhie_literal', 'korik', 'eme'}</t>
+          <t>{'andamhie_literal', 'chika_literal', 'korik', 'eme', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>{'==', '-', '&amp;&amp;', '&lt;=', '%', '*', '//', '||', '!=', '&gt;', '/', '+', '&gt;=', '&lt;', '**'}</t>
+          <t>{'*', '+', '&gt;=', '/', '==', '%', '&lt;=', '//', '**', '&gt;', '!=', '&amp;&amp;', '-', '&lt;', '||'}</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>{'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'id', 'serve', 'pak', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'andamhie', 'anda', 'keri', 'versa', 'forda', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'gogogo', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'id', 'serve', 'pak', 'gogogo', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'amaccana', 'andamhie', 'anda', 'keri', 'versa', 'forda', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'gogogo', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', 'gogogo', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'amaccana', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>{'/=', '//=', '*=', '(', '[', '%=', '=', '**=', '-=', '+='}</t>
+          <t>{'(', '/=', '+=', '*=', '**=', '[', '=', '//=', '-=', '%='}</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>{'/=', '%=', '//=', '=', '*=', '**=', '-=', '+='}</t>
+          <t>{'*=', '=', '**=', '+=', '/=', '//=', '-=', '%='}</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', '{', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '{', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>{'id', 'andamhie', 'anda', 'eklabool', 'chika'}</t>
+          <t>{'andamhie', 'id', 'anda', 'chika', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>{'andamhie', 'anda', 'eklabool', 'λ', 'chika'}</t>
+          <t>{'chika', 'andamhie', 'anda', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>{'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'gogogo', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', 'gogogo', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'amaccana', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>{'ganern', 'λ'}</t>
+          <t>{'λ', 'ganern'}</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>{'ganern', 'λ'}</t>
+          <t>{'λ', 'ganern'}</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>{'andamhie', 'anda', 'eklabool', 'λ', 'chika'}</t>
+          <t>{'chika', 'andamhie', 'anda', 'eklabool', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'λ', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', 'λ', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'gogogo', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', 'gogogo', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'amaccana', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>{'(', 'lang'}</t>
+          <t>{'lang', '('}</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'gogogo', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', 'gogogo', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'amaccana', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>{'λ', 'betsung'}</t>
+          <t>{'betsung', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>{'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>{'λ', 'betsung'}</t>
+          <t>{'betsung', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', '--', '++', 'adelete', 'pak', 'chika', 'forda', 'id', 'andamhie', 'versa', 'keri', 'serve', 'naur', 'gogogo', 'eklabool', 'adele', 'λ', 'anda'}</t>
+          <t>{'forda', 'id', 'pak', 'gogogo', '--', 'chika', 'push', 'eklabool', '++', 'λ', 'naur', 'adelete', 'amaccana', 'andamhie', 'anda', 'keri', 'versa', 'serve', 'adele'}</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>{'amaccana', 'λ', 'gogogo'}</t>
+          <t>{'amaccana', 'gogogo', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>{'λ', 'push'}</t>
+          <t>{'push', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>{'id', '--', '++'}</t>
+          <t>{'--', 'id', '++'}</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>{'-', 'id', 'anda_literal', 'chika_literal', '!', 'korik', 'andamhie_literal', 'len', '(', '--', '++', 'λ', 'eme'}</t>
+          <t>{'andamhie_literal', '(', 'id', 'len', 'korik', 'eme', 'λ', '--', 'chika_literal', '-', '!', '++', 'anda_literal'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: nested array as initializer of an array variable
</commit_message>
<xml_diff>
--- a/Files/cfg/first_set.xlsx
+++ b/Files/cfg/first_set.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'shimenet', 'andamhie', 'chika', 'naur'}</t>
+          <t>{'eklabool', 'andamhie', 'shimenet', 'chika', 'anda', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'shimenet', 'andamhie', 'chika', 'naur'}</t>
+          <t>{'eklabool', 'andamhie', 'shimenet', 'chika', 'anda', 'naur', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'shimenet', 'andamhie', 'chika', 'naur'}</t>
+          <t>{'eklabool', 'andamhie', 'chika', 'shimenet', 'anda', 'naur', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'shimenet', 'andamhie', 'chika'}</t>
+          <t>{'eklabool', 'anda', 'andamhie', 'chika', 'shimenet'}</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'andamhie', 'chika'}</t>
+          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{'[', 'λ', '(', '='}</t>
+          <t>{'(', 'λ', '[', '='}</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'andamhie', 'chika'}</t>
+          <t>{'eklabool', 'andamhie', 'anda', 'chika', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'andamhie', 'chika'}</t>
+          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{'[', 'λ'}</t>
+          <t>{'λ', '['}</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>{'[', 'λ'}</t>
+          <t>{'λ', '['}</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>{'[', 'λ'}</t>
+          <t>{'λ', '['}</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>{'[', 'λ'}</t>
+          <t>{'λ', '['}</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{'korik', 'chika_literal', 'eme', 'andamhie_literal', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'chika_literal', 'korik', 'anda_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>{'korik', 'eme'}</t>
+          <t>{'eme', 'korik'}</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{'[', 'λ', '('}</t>
+          <t>{'(', 'λ', '['}</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>{'[', 'λ', '('}</t>
+          <t>{'(', 'λ', '['}</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -987,7 +987,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', '{', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', '{', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'shimenet', 'andamhie', 'chika'}</t>
+          <t>{'eklabool', 'anda', 'andamhie', 'shimenet', 'chika', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'serve', 'forda', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'andamhie', 'chika', 'naur'}</t>
+          <t>{'eklabool', 'anda', 'naur', 'andamhie', 'chika', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'andamhie', 'chika', 'naur'}</t>
+          <t>{'eklabool', 'andamhie', 'chika', 'anda', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'λ', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'λ', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>{'id', 'λ'}</t>
+          <t>{'λ', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'serve', 'forda', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>{'*', 'λ', '==', '//', '&lt;=', '&amp;&amp;', '-', '&gt;', '&lt;', '&gt;=', '!=', '||', '/', '+', '%', '**'}</t>
+          <t>{'%', '!=', '**', '&gt;', '&lt;=', '&amp;&amp;', '==', '&lt;', '/', '&gt;=', '||', '-', 'λ', '*', '+', '//'}</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>{'λ', '-', '!'}</t>
+          <t>{'!', 'λ', '-'}</t>
         </is>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', 'eme', '(', 'id', 'andamhie_literal', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>{'λ', '++', '[', '(', '--'}</t>
+          <t>{'--', '(', 'λ', '[', '++'}</t>
         </is>
       </c>
     </row>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>{'++', '--'}</t>
+          <t>{'--', '++'}</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>{'korik', 'chika_literal', 'eme', 'andamhie_literal', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'chika_literal', 'korik', 'anda_literal', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>{'*', '==', '//', '&lt;=', '&amp;&amp;', '-', '&gt;', '&lt;', '&gt;=', '!=', '||', '/', '+', '%', '**'}</t>
+          <t>{'%', '!=', '**', '&gt;', '&lt;=', '&amp;&amp;', '==', '&lt;', '/', '&gt;=', '||', '-', '*', '+', '//'}</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'serve', 'forda', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'amaccana', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'gogogo', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'gogogo', 'serve', 'forda', 'amaccana', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'amaccana', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'gogogo', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'gogogo', 'serve', 'forda', 'amaccana', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>{'/=', '%=', '**=', '-=', '*=', '+=', '=', '[', '(', '//='}</t>
+          <t>{'**=', '//=', '%=', '[', '/=', '-=', '+=', '=', '(', '*='}</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>{'*=', '/=', '%=', '=', '**=', '-=', '+=', '//='}</t>
+          <t>{'+=', '=', '**=', '//=', '%=', '/=', '*=', '-='}</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', '{', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', '{', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'andamhie', 'chika', 'id'}</t>
+          <t>{'eklabool', 'andamhie', 'anda', 'id', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'andamhie', 'chika'}</t>
+          <t>{'eklabool', 'andamhie', 'anda', 'chika', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'serve', 'forda', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'amaccana', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'gogogo', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'gogogo', 'serve', 'forda', 'amaccana', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>{'ganern', 'λ'}</t>
+          <t>{'λ', 'ganern'}</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>{'ganern', 'λ'}</t>
+          <t>{'λ', 'ganern'}</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>{'anda', 'eklabool', 'λ', 'andamhie', 'chika'}</t>
+          <t>{'eklabool', 'andamhie', 'anda', 'chika', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>{'step', 'λ'}</t>
+          <t>{'λ', 'step'}</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'λ', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'λ', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'amaccana', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'gogogo', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'gogogo', 'serve', 'forda', 'amaccana', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'amaccana', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'gogogo', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'gogogo', 'serve', 'forda', 'amaccana', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>{'λ', 'betsung'}</t>
+          <t>{'betsung', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'len', '!', '-', 'andamhie_literal', 'eme', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'serve', 'forda', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>{'λ', 'betsung'}</t>
+          <t>{'betsung', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>{'++', 'forda', 'amaccana', 'keri', 'naur', 'adele', 'anda', 'eklabool', 'push', 'pak', 'λ', 'andamhie', 'adelete', 'chika', 'gogogo', 'versa', 'serve', 'id', '--'}</t>
+          <t>{'eklabool', 'id', 'keri', 'push', '++', 'anda', 'naur', 'adele', 'andamhie', '--', 'gogogo', 'serve', 'forda', 'amaccana', 'adelete', 'versa', 'chika', 'λ', 'pak'}</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>{'ditech', 'λ'}</t>
+          <t>{'λ', 'ditech'}</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>{'gogogo', 'amaccana', 'λ'}</t>
+          <t>{'amaccana', 'λ', 'gogogo'}</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>{'push', 'λ'}</t>
+          <t>{'λ', 'push'}</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>{'++', '--', 'id'}</t>
+          <t>{'--', '++', 'id'}</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>{'korik', '++', 'chika_literal', 'λ', 'len', '!', '-', 'andamhie_literal', 'eme', '{', 'id', '(', '--', 'anda_literal'}</t>
+          <t>{'andamhie_literal', 'len', '!', 'chika_literal', 'id', 'anda_literal', '--', '++', 'λ', '{', 'korik', '-', '(', 'eme'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Added array functions semantic
</commit_message>
<xml_diff>
--- a/Files/cfg/first_set.xlsx
+++ b/Files/cfg/first_set.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'chika', 'naur', 'eklabool', 'andamhie', 'shimenet', 'anda'}</t>
+          <t>{'chika', 'naur', 'shimenet', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'chika', 'naur', 'eklabool', 'andamhie', 'shimenet', 'λ', 'anda'}</t>
+          <t>{'chika', 'λ', 'naur', 'shimenet', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'chika', 'naur', 'eklabool', 'andamhie', 'shimenet', 'λ', 'anda'}</t>
+          <t>{'chika', 'λ', 'naur', 'shimenet', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{'naur', 'λ'}</t>
+          <t>{'λ', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'chika', 'anda', 'shimenet', 'eklabool', 'andamhie'}</t>
+          <t>{'chika', 'anda', 'andamhie', 'eklabool', 'shimenet'}</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{'chika', 'eklabool', 'andamhie', 'anda'}</t>
+          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{'=', '[', '(', 'λ'}</t>
+          <t>{'[', '(', '=', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>{'(', '['}</t>
+          <t>{'[', '('}</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{'chika', 'eklabool', 'andamhie', 'λ', 'anda'}</t>
+          <t>{'chika', 'λ', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{'eklabool', 'chika', 'anda', 'andamhie'}</t>
+          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{'λ', '['}</t>
+          <t>{'[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>{'λ', '['}</t>
+          <t>{'[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>{'λ', '['}</t>
+          <t>{'[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>{'λ', '['}</t>
+          <t>{'[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{'chika_literal', 'eme', 'anda_literal', 'korik', 'andamhie_literal'}</t>
+          <t>{'eme', 'chika_literal', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{'(', 'λ', '['}</t>
+          <t>{'(', '[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>{'[', '(', 'λ'}</t>
+          <t>{'(', '[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>{'=', 'λ'}</t>
+          <t>{'λ', '='}</t>
         </is>
       </c>
     </row>
@@ -927,7 +927,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>{'=', 'λ'}</t>
+          <t>{'λ', '='}</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -967,7 +967,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>{'=', 'λ'}</t>
+          <t>{'λ', '='}</t>
         </is>
       </c>
     </row>
@@ -987,7 +987,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', '{', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '{', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>{'andamhie', 'chika', 'anda', 'λ', 'eklabool', 'shimenet'}</t>
+          <t>{'chika', 'anda', 'λ', 'andamhie', 'eklabool', 'shimenet'}</t>
         </is>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'pak', 'forda', '--', 'adelete', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>{'chika', 'anda', 'λ', 'naur', 'eklabool', 'andamhie'}</t>
+          <t>{'chika', 'anda', 'λ', 'andamhie', 'eklabool', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>{'chika', 'naur', 'eklabool', 'andamhie', 'anda'}</t>
+          <t>{'chika', 'naur', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', 'λ', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', 'λ', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>{'id', 'λ'}</t>
+          <t>{'λ', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'pak', 'forda', '--', 'adelete', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>{'-', '==', '/', '&gt;=', '**', '&lt;=', '*', '!=', '+', '%', '&gt;', 'λ', '&lt;', '//', '&amp;&amp;', '||'}</t>
+          <t>{'&lt;=', '//', '%', '&gt;=', '||', '-', '!=', 'λ', '*', '**', '&lt;', '==', '&gt;', '/', '&amp;&amp;', '+'}</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>{'!', 'λ', '-'}</t>
+          <t>{'-', 'λ', '!'}</t>
         </is>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '(', '--', 'anda_literal', 'len', 'korik', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '(', '++', '--', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>{'λ', '[', '(', '--', '++'}</t>
+          <t>{'++', '--', '(', '[', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>{'chika_literal', 'eme', 'anda_literal', 'andamhie_literal', 'korik'}</t>
+          <t>{'eme', 'chika_literal', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>{'-', '==', '/', '&gt;=', '**', '&lt;=', '*', '!=', '+', '%', '&gt;', '&lt;', '//', '&amp;&amp;', '||'}</t>
+          <t>{'&lt;=', '//', '%', '&gt;=', '||', '-', '!=', '*', '**', '&lt;', '==', '&gt;', '/', '&amp;&amp;', '+'}</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'pak', 'forda', '--', 'adelete', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'gogogo', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'forda', 'pak', '--', 'adelete', 'eklabool', 'λ', 'anda', 'amaccana'}</t>
+          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'gogogo', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'forda', 'pak', '--', 'adelete', 'eklabool', 'λ', 'anda', 'amaccana'}</t>
+          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>{'//=', '[', '(', '+=', '/=', '-=', '**=', '*=', '%=', '='}</t>
+          <t>{'+=', '//=', '*=', '-=', '[', '**=', '(', '/=', '%=', '='}</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>{'//=', '*=', '**=', '+=', '=', '%=', '/=', '-='}</t>
+          <t>{'+=', '//=', '*=', '%=', '-=', '**=', '=', '/='}</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', '{', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '{', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>{'id', 'chika', 'anda', 'eklabool', 'andamhie'}</t>
+          <t>{'chika', 'anda', 'andamhie', 'id', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>{'chika', 'eklabool', 'andamhie', 'λ', 'anda'}</t>
+          <t>{'chika', 'λ', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'pak', 'forda', '--', 'adelete', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'gogogo', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'forda', 'pak', '--', 'adelete', 'eklabool', 'λ', 'anda', 'amaccana'}</t>
+          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>{'λ', 'ganern'}</t>
+          <t>{'ganern', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>{'λ', 'ganern'}</t>
+          <t>{'ganern', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>{'chika', 'eklabool', 'andamhie', 'λ', 'anda'}</t>
+          <t>{'chika', 'λ', 'anda', 'andamhie', 'eklabool'}</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>{'step', 'λ'}</t>
+          <t>{'λ', 'step'}</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', 'λ', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', 'λ', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'gogogo', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'forda', 'pak', '--', 'adelete', 'eklabool', 'λ', 'anda', 'amaccana'}</t>
+          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>{'lang', '('}</t>
+          <t>{'(', 'lang'}</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'gogogo', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'forda', 'pak', '--', 'adelete', 'eklabool', 'λ', 'anda', 'amaccana'}</t>
+          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>{'betsung', 'λ'}</t>
+          <t>{'λ', 'betsung'}</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', 'len', 'korik', '!', 'chika_literal', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'pak', 'forda', '--', 'adelete', 'eklabool', 'λ', 'anda'}</t>
+          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>{'betsung', 'λ'}</t>
+          <t>{'λ', 'betsung'}</t>
         </is>
       </c>
     </row>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>{'naur', 'andamhie', 'push', 'keri', 'gogogo', 'serve', '++', 'id', 'versa', 'adele', 'chika', 'forda', 'pak', '--', 'adelete', 'eklabool', 'λ', 'anda', 'amaccana'}</t>
+          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>{'ditech', 'λ'}</t>
+          <t>{'λ', 'ditech'}</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>{'gogogo', 'amaccana', 'λ'}</t>
+          <t>{'λ', 'amaccana', 'gogogo'}</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>{'id', 'eme', '-', '(', '--', 'anda_literal', '{', 'len', 'korik', '!', 'chika_literal', 'λ', '++', 'andamhie_literal'}</t>
+          <t>{'eme', 'len', '-', '(', 'λ', '++', '--', '{', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: cfg array indexing fix
</commit_message>
<xml_diff>
--- a/Files/cfg/first_set.xlsx
+++ b/Files/cfg/first_set.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'chika', 'naur', 'shimenet', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'andamhie', 'chika', 'shimenet', 'eklabool', 'anda', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'chika', 'λ', 'naur', 'shimenet', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'andamhie', 'chika', 'shimenet', 'eklabool', 'anda', 'λ', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'chika', 'λ', 'naur', 'shimenet', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'andamhie', 'chika', 'shimenet', 'eklabool', 'anda', 'λ', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'chika', 'anda', 'andamhie', 'eklabool', 'shimenet'}</t>
+          <t>{'shimenet', 'eklabool', 'anda', 'andamhie', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
+          <t>{'chika', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{'[', '(', '=', 'λ'}</t>
+          <t>{'[', 'λ', '(', '='}</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{'chika', 'λ', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'andamhie', 'chika', 'eklabool', 'anda', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{'andamhie', 'eklabool', 'chika', 'anda'}</t>
+          <t>{'chika', 'eklabool', 'anda', 'andamhie'}</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{'λ', ','}</t>
+          <t>{',', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>First(&lt;2d-index&gt;)</t>
+          <t>First(&lt;multi-index&gt;)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>First(&lt;3d-index&gt;)</t>
+          <t>First(&lt;array-values&gt;)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>{'[', 'λ'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>First(&lt;array-values&gt;)</t>
+          <t>First(&lt;literals&gt;)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'anda_literal', 'andamhie_literal', 'chika_literal', 'korik', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>First(&lt;literals&gt;)</t>
+          <t>First(&lt;eklabool&gt;)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'korik', 'eme'}</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>First(&lt;eklabool&gt;)</t>
+          <t>First(&lt;func-array&gt;)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>{'eme', 'korik'}</t>
+          <t>{'[', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -817,7 +817,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>First(&lt;func-array&gt;)</t>
+          <t>First(&lt;func-array-value&gt;)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{'(', '[', 'λ'}</t>
+          <t>{'[', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>First(&lt;func-array-value&gt;)</t>
+          <t>First(&lt;var-init&gt;)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>{'(', '[', 'λ'}</t>
+          <t>{'id'}</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>First(&lt;var-init&gt;)</t>
+          <t>First(&lt;var-init-tail&gt;)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>{'id'}</t>
+          <t>{'λ', '='}</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>First(&lt;var-init-tail&gt;)</t>
+          <t>First(&lt;multi-init-values&gt;)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>{'λ', '='}</t>
+          <t>{',', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>First(&lt;multi-init-values&gt;)</t>
+          <t>First(&lt;multi-init-values-tail&gt;)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>{'λ', ','}</t>
+          <t>{'λ', '='}</t>
         </is>
       </c>
     </row>
@@ -917,7 +917,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>First(&lt;multi-init-values-tail&gt;)</t>
+          <t>First(&lt;init-values&gt;)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>{'λ', '='}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>First(&lt;init-values&gt;)</t>
+          <t>First(&lt;array-init&gt;)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -947,7 +947,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'λ', '='}</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>First(&lt;array-init&gt;)</t>
+          <t>First(&lt;array-elements&gt;)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>{'λ', '='}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', '{', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -977,7 +977,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>First(&lt;array-elements&gt;)</t>
+          <t>First(&lt;extra-array-value&gt;)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '{', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{',', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>First(&lt;extra-array-value&gt;)</t>
+          <t>First(&lt;func-def&gt;)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>{'λ', ','}</t>
+          <t>{'shimenet', 'eklabool', 'anda', 'andamhie', 'λ', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>First(&lt;func-def&gt;)</t>
+          <t>First(&lt;func-body&gt;)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>{'chika', 'anda', 'λ', 'andamhie', 'eklabool', 'shimenet'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>First(&lt;func-body&gt;)</t>
+          <t>First(&lt;local-dec&gt;)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'eklabool', 'anda', 'andamhie', 'λ', 'chika', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>First(&lt;local-dec&gt;)</t>
+          <t>First(&lt;local-dec-init&gt;)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>{'chika', 'anda', 'λ', 'andamhie', 'eklabool', 'naur'}</t>
+          <t>{'andamhie', 'chika', 'eklabool', 'anda', 'naur'}</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>First(&lt;local-dec-init&gt;)</t>
+          <t>First(&lt;arguments&gt;)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>{'chika', 'naur', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>First(&lt;arguments&gt;)</t>
+          <t>First(&lt;multi-arguments-value&gt;)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', 'λ', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{',', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>First(&lt;multi-arguments-value&gt;)</t>
+          <t>First(&lt;arguments-value&gt;)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>{'λ', ','}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>First(&lt;arguments-value&gt;)</t>
+          <t>First(&lt;array-assign&gt;)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'id', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>First(&lt;array-assign&gt;)</t>
+          <t>First(&lt;kween-body&gt;)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>{'λ', 'id'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>First(&lt;kween-body&gt;)</t>
+          <t>First(&lt;expression&gt;)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>First(&lt;expression&gt;)</t>
+          <t>First(&lt;simple-expression&gt;)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>First(&lt;simple-expression&gt;)</t>
+          <t>First(&lt;multi-expression&gt;)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'('}</t>
         </is>
       </c>
     </row>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>First(&lt;multi-expression&gt;)</t>
+          <t>First(&lt;expression-tail&gt;)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>{'('}</t>
+          <t>{'&lt;=', '!=', '%', '&gt;', '&lt;', '/', '*', '-', '**', '||', '//', '&gt;=', '==', '&amp;&amp;', '+', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>First(&lt;expression-tail&gt;)</t>
+          <t>First(&lt;expression-operands&gt;)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>{'&lt;=', '//', '%', '&gt;=', '||', '-', '!=', 'λ', '*', '**', '&lt;', '==', '&gt;', '/', '&amp;&amp;', '+'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>First(&lt;expression-operands&gt;)</t>
+          <t>First(&lt;negative-not-value&gt;)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'!', 'λ', '-'}</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>First(&lt;negative-not-value&gt;)</t>
+          <t>First(&lt;expression-value&gt;)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>{'-', 'λ', '!'}</t>
+          <t>{'anda_literal', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>First(&lt;expression-value&gt;)</t>
+          <t>First(&lt;len-choice&gt;)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '(', '++', '--', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'id', 'chika_literal'}</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>First(&lt;len-choice&gt;)</t>
+          <t>First(&lt;identifier-tail&gt;)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>{'id', 'chika_literal'}</t>
+          <t>{'++', '[', '--', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>First(&lt;identifier-tail&gt;)</t>
+          <t>First(&lt;unary-operator&gt;)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>{'++', '--', '(', '[', 'λ'}</t>
+          <t>{'--', '++'}</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>First(&lt;unary-operator&gt;)</t>
+          <t>First(&lt;general-operands&gt;)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>{'++', '--'}</t>
+          <t>{'anda_literal', 'chika_literal', 'andamhie_literal', 'eme', 'korik'}</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>First(&lt;general-operands&gt;)</t>
+          <t>First(&lt;general-operators&gt;)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>{'eme', 'chika_literal', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'&lt;=', '!=', '%', '&gt;', '&lt;', '/', '*', '-', '**', '||', '//', '&gt;=', '==', '&amp;&amp;', '+'}</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>First(&lt;general-operators&gt;)</t>
+          <t>First(&lt;statements&gt;)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>{'&lt;=', '//', '%', '&gt;=', '||', '-', '!=', '*', '**', '&lt;', '==', '&gt;', '/', '&amp;&amp;', '+'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>First(&lt;statements&gt;)</t>
+          <t>First(&lt;loop-body&gt;)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'gogogo', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'amaccana', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>First(&lt;loop-body&gt;)</t>
+          <t>First(&lt;multi-loop-body&gt;)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'gogogo', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'amaccana', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>First(&lt;multi-loop-body&gt;)</t>
+          <t>First(&lt;assign-call-stmts&gt;)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1487,7 +1487,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'//=', '[', '**=', '=', '*=', '+=', '/=', '-=', '(', '%='}</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>First(&lt;assign-call-stmts&gt;)</t>
+          <t>First(&lt;assignment-operators&gt;)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>{'+=', '//=', '*=', '-=', '[', '**=', '(', '/=', '%=', '='}</t>
+          <t>{'=', '*=', '+=', '/=', '//=', '-=', '%=', '**='}</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>First(&lt;assignment-operators&gt;)</t>
+          <t>First(&lt;assignment-values&gt;)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>{'+=', '//=', '*=', '%=', '-=', '**=', '=', '/='}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', '{', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>First(&lt;assignment-values&gt;)</t>
+          <t>First(&lt;input-stmts&gt;)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '{', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'eklabool', 'anda', 'andamhie', 'id', 'chika'}</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>First(&lt;input-stmts&gt;)</t>
+          <t>First(&lt;input-type&gt;)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>{'chika', 'anda', 'andamhie', 'id', 'eklabool'}</t>
+          <t>{'andamhie', 'chika', 'eklabool', 'anda', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>First(&lt;input-type&gt;)</t>
+          <t>First(&lt;givenchy-values&gt;)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>{'chika', 'λ', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>First(&lt;givenchy-values&gt;)</t>
+          <t>First(&lt;output-stmts&gt;)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'serve'}</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>First(&lt;output-stmts&gt;)</t>
+          <t>First(&lt;append-stmts&gt;)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>{'serve'}</t>
+          <t>{'adele'}</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>First(&lt;append-stmts&gt;)</t>
+          <t>First(&lt;delete-stmts&gt;)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>{'adele'}</t>
+          <t>{'adelete'}</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>First(&lt;delete-stmts&gt;)</t>
+          <t>First(&lt;output-values&gt;)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>{'adelete'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>First(&lt;output-values&gt;)</t>
+          <t>First(&lt;conditional-stmts&gt;)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'pak'}</t>
         </is>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>First(&lt;conditional-stmts&gt;)</t>
+          <t>First(&lt;condition&gt;)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>{'pak'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>First(&lt;condition&gt;)</t>
+          <t>First(&lt;conditional-body&gt;)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>First(&lt;conditional-body&gt;)</t>
+          <t>First(&lt;loop-conditional-stmts&gt;)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'pak'}</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>First(&lt;loop-conditional-stmts&gt;)</t>
+          <t>First(&lt;loop-conditional-body&gt;)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>{'pak'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'gogogo', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'amaccana', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>First(&lt;loop-conditional-body&gt;)</t>
+          <t>First(&lt;ganern-pak-statement&gt;)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'ganern', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>First(&lt;ganern-pak-statement&gt;)</t>
+          <t>First(&lt;ganern-case&gt;)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>First(&lt;ganern-case&gt;)</t>
+          <t>First(&lt;loop-stmts&gt;)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>{'ganern', 'λ'}</t>
+          <t>{'forda', 'keri'}</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>First(&lt;loop-stmts&gt;)</t>
+          <t>First(&lt;forda-statement&gt;)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>{'keri', 'forda'}</t>
+          <t>{'forda'}</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>First(&lt;forda-statement&gt;)</t>
+          <t>First(&lt;loop-type-init&gt;)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>{'forda'}</t>
+          <t>{'andamhie', 'chika', 'eklabool', 'anda', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>First(&lt;loop-type-init&gt;)</t>
+          <t>First(&lt;start-value&gt;)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1887,7 +1887,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>{'chika', 'λ', 'anda', 'andamhie', 'eklabool'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>First(&lt;start-value&gt;)</t>
+          <t>First(&lt;end-value&gt;)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>First(&lt;end-value&gt;)</t>
+          <t>First(&lt;step-case&gt;)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'step', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>First(&lt;step-case&gt;)</t>
+          <t>First(&lt;update&gt;)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>{'λ', 'step'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>First(&lt;update&gt;)</t>
+          <t>First(&lt;loop-conditions&gt;)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', 'λ', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>First(&lt;loop-conditions&gt;)</t>
+          <t>First(&lt;for-loop-body&gt;)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'gogogo', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'amaccana', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>First(&lt;for-loop-body&gt;)</t>
+          <t>First(&lt;keri-statement&gt;)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2007,7 +2007,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'keri'}</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>First(&lt;keri-statement&gt;)</t>
+          <t>First(&lt;keri-case&gt;)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>{'keri'}</t>
+          <t>{'(', 'lang'}</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>First(&lt;keri-case&gt;)</t>
+          <t>First(&lt;while-loop-body&gt;)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>{'(', 'lang'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'gogogo', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'amaccana', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>First(&lt;while-loop-body&gt;)</t>
+          <t>First(&lt;switch-stmts&gt;)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'versa'}</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>First(&lt;switch-stmts&gt;)</t>
+          <t>First(&lt;multi-cases&gt;)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>{'versa'}</t>
+          <t>{'betsung', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>First(&lt;multi-cases&gt;)</t>
+          <t>First(&lt;switch-values&gt;)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>{'λ', 'betsung'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', 'chika_literal', '('}</t>
         </is>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>First(&lt;switch-values&gt;)</t>
+          <t>First(&lt;switch-statements&gt;)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>{'eme', 'len', '-', '(', '++', '--', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>First(&lt;switch-statements&gt;)</t>
+          <t>First(&lt;loop-switch-stmts&gt;)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>{'push', 'λ', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'versa'}</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>First(&lt;loop-switch-stmts&gt;)</t>
+          <t>First(&lt;loop-multi-cases&gt;)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>{'versa'}</t>
+          <t>{'betsung', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>First(&lt;loop-multi-cases&gt;)</t>
+          <t>First(&lt;loop-switch-statements&gt;)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>{'λ', 'betsung'}</t>
+          <t>{'versa', '++', 'adelete', 'andamhie', 'id', 'push', '--', 'gogogo', 'eklabool', 'anda', 'serve', 'λ', 'pak', 'chika', 'amaccana', 'keri', 'adele', 'naur', 'forda'}</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>First(&lt;loop-switch-statements&gt;)</t>
+          <t>First(&lt;amaccana-case&gt;)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>{'amaccana', 'push', 'λ', 'gogogo', 'keri', 'naur', '++', '--', 'adele', 'adelete', 'eklabool', 'forda', 'chika', 'serve', 'pak', 'versa', 'anda', 'andamhie', 'id'}</t>
+          <t>{'λ', 'amaccana'}</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>First(&lt;amaccana-case&gt;)</t>
+          <t>First(&lt;ditech-case&gt;)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>{'λ', 'amaccana'}</t>
+          <t>{'λ', 'ditech'}</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>First(&lt;ditech-case&gt;)</t>
+          <t>First(&lt;control-flow-stmts&gt;)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>{'λ', 'ditech'}</t>
+          <t>{'gogogo', 'λ', 'amaccana'}</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>First(&lt;control-flow-stmts&gt;)</t>
+          <t>First(&lt;return-stmts&gt;)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>{'λ', 'amaccana', 'gogogo'}</t>
+          <t>{'push', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>First(&lt;return-stmts&gt;)</t>
+          <t>First(&lt;unary-stmts&gt;)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>{'λ', 'push'}</t>
+          <t>{'id', '--', '++'}</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>First(&lt;unary-stmts&gt;)</t>
+          <t>First(&lt;push-values&gt;)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>{'id', '++', '--'}</t>
+          <t>{'anda_literal', '!', '++', 'id', 'andamhie_literal', '--', 'korik', 'eme', 'len', '-', '{', 'chika_literal', '(', 'λ'}</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>First(&lt;push-values&gt;)</t>
+          <t>First()</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2326,26 +2326,6 @@
         </is>
       </c>
       <c r="D95" t="inlineStr">
-        <is>
-          <t>{'eme', 'len', '-', '(', 'λ', '++', '--', '{', '!', 'chika_literal', 'id', 'korik', 'anda_literal', 'andamhie_literal'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>95</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>First()</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>-&gt;</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
         <is>
           <t>set()</t>
         </is>

</xml_diff>